<commit_message>
finished updating topic 2
</commit_message>
<xml_diff>
--- a/topic_1_img/Topic 1 Example.xlsx
+++ b/topic_1_img/Topic 1 Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u167856\Dropbox\UPF\managerial_accounting\2023-2024\Slides\topic_1_img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE893513-3906-4906-978B-A473FE6DEEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33486258-6B13-4D09-ABA0-C7E97F6CD053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejemplo 1" sheetId="1" r:id="rId1"/>
@@ -261,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0_-;\-[$€-2]\ * #,##0_-;_-[$€-2]\ * \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +296,41 @@
     <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -411,21 +446,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -495,6 +521,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,1087 +816,1087 @@
   <dimension ref="B2:T66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="9.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="4" customWidth="1"/>
-    <col min="12" max="13" width="15.33203125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="21.88671875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" style="4" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="1.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="9.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="15.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17" style="2" customWidth="1"/>
     <col min="19" max="19" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="30"/>
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="5" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="T3" s="6" t="s">
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="T3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="1"/>
+      <c r="D4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="T4" s="6"/>
+      <c r="T4" s="3"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>30000</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4">
         <v>30000</v>
       </c>
-      <c r="R5" s="7"/>
+      <c r="R5" s="4"/>
       <c r="T5" t="str">
         <f t="shared" ref="T5:T19" si="0">IF(SUM(D5:I5)=SUM(K5:R5)," ","Error")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>-20000</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <v>20000</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
       <c r="T6" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
         <v>-200</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="5">
         <v>-200</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
       <c r="T7" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
         <v>500</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>500</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
       <c r="T8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>-500</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
         <v>-500</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
       <c r="T9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
         <v>-500</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4">
         <v>-500</v>
       </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
       <c r="T10" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>4</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>5500</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4">
         <v>5500</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
       <c r="T11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4">
         <v>600</v>
       </c>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="5">
         <v>-600</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
       <c r="T12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>5</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
         <v>3000</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4">
         <v>3000</v>
       </c>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
       <c r="T13" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4">
         <v>200</v>
       </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="8">
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5">
         <v>-200</v>
       </c>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
       <c r="T14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>6</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>-1100</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="8">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="5">
         <v>-1100</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
       <c r="T15" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>-1600</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="8">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="5">
         <v>-1600</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
       <c r="T16" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>7</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>5000</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4">
         <v>5000</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
       <c r="T17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9">
+      <c r="C18" s="1"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6">
         <v>35</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9">
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6">
         <v>-35</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
       <c r="T18" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <f t="shared" ref="D19:R19" si="1">SUM(D5:D18)</f>
         <v>17300</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="4">
         <f t="shared" si="1"/>
         <v>19800</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="4">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="4">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="4">
         <f t="shared" si="1"/>
         <v>8500</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="4">
         <f t="shared" si="1"/>
         <v>-4235</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="4">
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S19" s="7"/>
+      <c r="S19" s="4"/>
       <c r="T19" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-    </row>
-    <row r="22" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-    </row>
-    <row r="23" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="1" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+    </row>
+    <row r="23" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="J23" s="1" t="s">
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="J23" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="12"/>
-      <c r="H24" s="13"/>
-      <c r="J24" s="12"/>
-      <c r="O24" s="13"/>
-    </row>
-    <row r="25" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="14" t="s">
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+      <c r="H24" s="10"/>
+      <c r="J24" s="9"/>
+      <c r="O24" s="10"/>
+    </row>
+    <row r="25" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="J25" s="14" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="J25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="16"/>
-    </row>
-    <row r="26" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="17" t="s">
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="13"/>
+    </row>
+    <row r="26" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="15">
         <f>+H27+H33</f>
         <v>40100</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="16">
         <f>+O19</f>
         <v>8500</v>
       </c>
     </row>
-    <row r="27" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="20" t="s">
+    <row r="27" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22">
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19">
         <f>+H28+H29+H30+H31</f>
         <v>20300</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O27" s="23">
+      <c r="O27" s="20">
         <f>+P14+P12</f>
         <v>-800</v>
       </c>
     </row>
-    <row r="28" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="12"/>
-      <c r="E28" s="10" t="s">
+    <row r="28" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="9"/>
+      <c r="E28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="16">
         <f>+D19</f>
         <v>17300</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="18">
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="15">
         <f>+O26+O27</f>
         <v>7700</v>
       </c>
     </row>
-    <row r="29" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="12"/>
-      <c r="E29" s="10" t="s">
+    <row r="29" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="9"/>
+      <c r="E29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="16">
         <f>+E19</f>
         <v>3000</v>
       </c>
-      <c r="J29" s="12"/>
-      <c r="O29" s="19"/>
-    </row>
-    <row r="30" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="12"/>
-      <c r="E30" s="10" t="s">
+      <c r="J29" s="9"/>
+      <c r="O29" s="16"/>
+    </row>
+    <row r="30" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="9"/>
+      <c r="E30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="J30" s="12" t="s">
+      <c r="H30" s="16"/>
+      <c r="J30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="16">
         <f>+SUM(O31:O37)</f>
         <v>-1800</v>
       </c>
     </row>
-    <row r="31" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="12"/>
-      <c r="E31" s="10" t="s">
+    <row r="31" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="9"/>
+      <c r="E31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="10" t="s">
+      <c r="H31" s="16"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O31" s="13"/>
-    </row>
-    <row r="32" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="12"/>
-      <c r="H32" s="19"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="10" t="s">
+      <c r="O31" s="10"/>
+    </row>
+    <row r="32" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="9"/>
+      <c r="H32" s="16"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="16">
         <f>+P7</f>
         <v>-200</v>
       </c>
     </row>
-    <row r="33" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="20" t="s">
+    <row r="33" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="22">
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19">
         <f>+H34+H35+H36</f>
         <v>19800</v>
       </c>
-      <c r="J33" s="12"/>
-      <c r="K33" s="10" t="s">
+      <c r="J33" s="9"/>
+      <c r="K33" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O33" s="19">
+      <c r="O33" s="16">
         <f>+P15</f>
         <v>-1100</v>
       </c>
     </row>
-    <row r="34" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="12"/>
-      <c r="E34" s="10" t="s">
+    <row r="34" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="9"/>
+      <c r="E34" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="16">
         <f>+H19</f>
         <v>19800</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="10" t="s">
+      <c r="J34" s="9"/>
+      <c r="K34" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O34" s="13"/>
-    </row>
-    <row r="35" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="12"/>
-      <c r="E35" s="10" t="s">
+      <c r="O34" s="10"/>
+    </row>
+    <row r="35" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="9"/>
+      <c r="E35" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="10" t="s">
+      <c r="H35" s="16"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="O35" s="13"/>
-    </row>
-    <row r="36" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="12"/>
-      <c r="E36" s="10" t="s">
+      <c r="O35" s="10"/>
+    </row>
+    <row r="36" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="9"/>
+      <c r="E36" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="10" t="s">
+      <c r="H36" s="16"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O36" s="19">
+      <c r="O36" s="16">
         <f>+P10</f>
         <v>-500</v>
       </c>
     </row>
-    <row r="37" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="12"/>
-      <c r="H37" s="19"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="10" t="s">
+    <row r="37" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="9"/>
+      <c r="H37" s="16"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O37" s="13"/>
-    </row>
-    <row r="38" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="12"/>
-      <c r="H38" s="19"/>
-      <c r="J38" s="12" t="s">
+      <c r="O37" s="10"/>
+    </row>
+    <row r="38" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="9"/>
+      <c r="H38" s="16"/>
+      <c r="J38" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="O38" s="25">
+      <c r="O38" s="22">
         <f>P16</f>
         <v>-1600</v>
       </c>
     </row>
-    <row r="39" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="17" t="s">
+    <row r="39" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="18">
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="15">
         <f>+H40+H46+H51</f>
         <v>40100</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="24"/>
-      <c r="O39" s="18">
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="15">
         <f>+O28+O30+O38</f>
         <v>4300</v>
       </c>
     </row>
-    <row r="40" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="12" t="s">
+    <row r="40" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="19">
+      <c r="H40" s="16">
         <f>+H41+H42+H43+H44</f>
         <v>835</v>
       </c>
-      <c r="J40" s="12"/>
-      <c r="O40" s="22"/>
-    </row>
-    <row r="41" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="12"/>
-      <c r="E41" s="10" t="s">
+      <c r="J40" s="9"/>
+      <c r="O40" s="19"/>
+    </row>
+    <row r="41" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="9"/>
+      <c r="E41" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="J41" s="12" t="s">
+      <c r="H41" s="16"/>
+      <c r="J41" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="O41" s="19"/>
-    </row>
-    <row r="42" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="12"/>
-      <c r="E42" s="10" t="s">
+      <c r="O41" s="16"/>
+    </row>
+    <row r="42" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="9"/>
+      <c r="E42" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H42" s="19">
+      <c r="H42" s="16">
         <f>+L19</f>
         <v>35</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="O42" s="26">
+      <c r="O42" s="23">
         <f>+P18</f>
         <v>-35</v>
       </c>
     </row>
-    <row r="43" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="12"/>
-      <c r="E43" s="10" t="s">
+    <row r="43" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="9"/>
+      <c r="E43" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="19"/>
-      <c r="J43" s="17" t="s">
+      <c r="H43" s="16"/>
+      <c r="J43" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="18">
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="15">
         <f>+O42</f>
         <v>-35</v>
       </c>
     </row>
-    <row r="44" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="12"/>
-      <c r="E44" s="10" t="s">
+    <row r="44" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="9"/>
+      <c r="E44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H44" s="19">
+      <c r="H44" s="16">
         <f>+M19</f>
         <v>800</v>
       </c>
-      <c r="J44" s="12"/>
-      <c r="O44" s="19"/>
-    </row>
-    <row r="45" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="12"/>
-      <c r="H45" s="19"/>
-      <c r="J45" s="12" t="s">
+      <c r="J44" s="9"/>
+      <c r="O44" s="16"/>
+    </row>
+    <row r="45" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="9"/>
+      <c r="H45" s="16"/>
+      <c r="J45" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="O45" s="19">
+      <c r="O45" s="16">
         <f>+O39+O43</f>
         <v>4265</v>
       </c>
     </row>
-    <row r="46" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="12" t="s">
+    <row r="46" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H46" s="19">
+      <c r="H46" s="16">
         <f>+H47+H48+H49</f>
         <v>5000</v>
       </c>
-      <c r="J46" s="12" t="s">
+      <c r="J46" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="O46" s="27"/>
-    </row>
-    <row r="47" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="12"/>
-      <c r="E47" s="10" t="s">
+      <c r="O46" s="24"/>
+    </row>
+    <row r="47" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="9"/>
+      <c r="E47" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="16">
         <f>+N19</f>
         <v>5000</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="18">
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="15">
         <f>+O45</f>
         <v>4265</v>
       </c>
     </row>
-    <row r="48" spans="4:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="12"/>
-      <c r="E48" s="10" t="s">
+    <row r="48" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="9"/>
+      <c r="E48" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H48" s="19"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="16"/>
-    </row>
-    <row r="49" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="12"/>
-      <c r="E49" s="10" t="s">
+      <c r="H48" s="16"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="13"/>
+    </row>
+    <row r="49" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="9"/>
+      <c r="E49" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="19"/>
-    </row>
-    <row r="50" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="12"/>
-      <c r="H50" s="19"/>
-    </row>
-    <row r="51" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="28" t="s">
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="9"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H51" s="19">
+      <c r="H51" s="16">
         <f>+H52+H53</f>
         <v>34265</v>
       </c>
     </row>
-    <row r="52" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="12"/>
-      <c r="E52" s="10" t="s">
+    <row r="52" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="9"/>
+      <c r="E52" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="19">
+      <c r="H52" s="16">
         <f>+Q19</f>
         <v>30000</v>
       </c>
     </row>
-    <row r="53" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="12"/>
-      <c r="E53" s="10" t="s">
+    <row r="53" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="9"/>
+      <c r="E53" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="19">
+      <c r="H53" s="16">
         <f>+O19+P19</f>
         <v>4265</v>
       </c>
     </row>
-    <row r="54" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="14"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="29"/>
-    </row>
-    <row r="55" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="4:8" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="11"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="4:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D3:G3"/>

</xml_diff>